<commit_message>
added surefire plugin pom.xml
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/simple.xlsx
+++ b/target/test-classes/testdata/simple.xlsx
@@ -16,12 +16,11 @@
     <sheet name="testData" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:R17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Username</t>
   </si>
@@ -81,19 +80,35 @@
   </si>
   <si>
     <t>lastaname</t>
+  </si>
+  <si>
+    <t>verifyLoginWithValidCred</t>
+  </si>
+  <si>
+    <t>w2ajava@way2automation.com</t>
+  </si>
+  <si>
+    <t>Tcs@12345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,13 +128,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -609,10 +630,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -687,7 +708,31 @@
         <v>16</v>
       </c>
     </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>